<commit_message>
PCA and clustering exploration
</commit_message>
<xml_diff>
--- a/data/Smart_Summit_Exact_Data_Export.xlsx
+++ b/data/Smart_Summit_Exact_Data_Export.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="16275" windowHeight="8760"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="28560" windowHeight="16780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -5931,9 +5936,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6061,7 +6066,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -6189,7 +6194,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -6317,7 +6322,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42">
       <c r="A4" s="1" t="s">
         <v>74</v>
       </c>
@@ -6445,7 +6450,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42">
       <c r="A5" s="1" t="s">
         <v>94</v>
       </c>
@@ -6573,7 +6578,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42">
       <c r="A6" s="1" t="s">
         <v>113</v>
       </c>
@@ -6701,7 +6706,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42">
       <c r="A7" s="1" t="s">
         <v>127</v>
       </c>
@@ -6829,7 +6834,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42">
       <c r="A8" s="1" t="s">
         <v>143</v>
       </c>
@@ -6957,7 +6962,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42">
       <c r="A9" s="1" t="s">
         <v>162</v>
       </c>
@@ -7085,7 +7090,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42">
       <c r="A10" s="1" t="s">
         <v>178</v>
       </c>
@@ -7213,7 +7218,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42">
       <c r="A11" s="1" t="s">
         <v>187</v>
       </c>
@@ -7341,7 +7346,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42">
       <c r="A12" s="1" t="s">
         <v>205</v>
       </c>
@@ -7469,7 +7474,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42">
       <c r="A13" s="1" t="s">
         <v>219</v>
       </c>
@@ -7597,7 +7602,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42">
       <c r="A14" s="1" t="s">
         <v>233</v>
       </c>
@@ -7725,7 +7730,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42">
       <c r="A15" s="1" t="s">
         <v>243</v>
       </c>
@@ -7853,7 +7858,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42">
       <c r="A16" s="1" t="s">
         <v>263</v>
       </c>
@@ -7981,7 +7986,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42">
       <c r="A17" s="1" t="s">
         <v>279</v>
       </c>
@@ -8109,7 +8114,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42">
       <c r="A18" s="1" t="s">
         <v>293</v>
       </c>
@@ -8237,7 +8242,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42">
       <c r="A19" s="1" t="s">
         <v>295</v>
       </c>
@@ -8365,7 +8370,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42">
       <c r="A20" s="1" t="s">
         <v>308</v>
       </c>
@@ -8493,7 +8498,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42">
       <c r="A21" s="1" t="s">
         <v>327</v>
       </c>
@@ -8621,7 +8626,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42">
       <c r="A22" s="1" t="s">
         <v>342</v>
       </c>
@@ -8749,7 +8754,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42">
       <c r="A23" s="1" t="s">
         <v>359</v>
       </c>
@@ -8877,7 +8882,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42">
       <c r="A24" s="1" t="s">
         <v>369</v>
       </c>
@@ -9005,7 +9010,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42">
       <c r="A25" s="1" t="s">
         <v>378</v>
       </c>
@@ -9133,7 +9138,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42">
       <c r="A26" s="1" t="s">
         <v>392</v>
       </c>
@@ -9261,7 +9266,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42">
       <c r="A27" s="1" t="s">
         <v>407</v>
       </c>
@@ -9389,7 +9394,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42">
       <c r="A28" s="1" t="s">
         <v>420</v>
       </c>
@@ -9517,7 +9522,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42">
       <c r="A29" s="1" t="s">
         <v>435</v>
       </c>
@@ -9645,7 +9650,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42">
       <c r="A30" s="1" t="s">
         <v>448</v>
       </c>
@@ -9773,7 +9778,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42">
       <c r="A31" s="1" t="s">
         <v>458</v>
       </c>
@@ -9901,7 +9906,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42">
       <c r="A32" s="1" t="s">
         <v>477</v>
       </c>
@@ -10029,7 +10034,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:42">
       <c r="A33" s="1" t="s">
         <v>493</v>
       </c>
@@ -10157,7 +10162,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:42">
       <c r="A34" s="1" t="s">
         <v>504</v>
       </c>
@@ -10285,7 +10290,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42">
       <c r="A35" s="1" t="s">
         <v>515</v>
       </c>
@@ -10413,7 +10418,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42">
       <c r="A36" s="1" t="s">
         <v>524</v>
       </c>
@@ -10541,7 +10546,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42">
       <c r="A37" s="1" t="s">
         <v>534</v>
       </c>
@@ -10669,7 +10674,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:42">
       <c r="A38" s="1" t="s">
         <v>546</v>
       </c>
@@ -10797,7 +10802,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:42">
       <c r="A39" s="1" t="s">
         <v>559</v>
       </c>
@@ -10925,7 +10930,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:42">
       <c r="A40" s="1" t="s">
         <v>573</v>
       </c>
@@ -11053,7 +11058,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:42">
       <c r="A41" s="1" t="s">
         <v>589</v>
       </c>
@@ -11181,7 +11186,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:42">
       <c r="A42" s="1" t="s">
         <v>598</v>
       </c>
@@ -11309,7 +11314,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:42">
       <c r="A43" s="1" t="s">
         <v>611</v>
       </c>
@@ -11437,7 +11442,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:42">
       <c r="A44" s="1" t="s">
         <v>624</v>
       </c>
@@ -11565,7 +11570,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:42">
       <c r="A45" s="1" t="s">
         <v>634</v>
       </c>
@@ -11693,7 +11698,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:42">
       <c r="A46" s="1" t="s">
         <v>646</v>
       </c>
@@ -11821,7 +11826,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:42">
       <c r="A47" s="1" t="s">
         <v>660</v>
       </c>
@@ -11949,7 +11954,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:42">
       <c r="A48" s="1" t="s">
         <v>669</v>
       </c>
@@ -12077,7 +12082,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:42">
       <c r="A49" s="1" t="s">
         <v>680</v>
       </c>
@@ -12205,7 +12210,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:42">
       <c r="A50" s="1" t="s">
         <v>694</v>
       </c>
@@ -12333,7 +12338,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:42">
       <c r="A51" s="1" t="s">
         <v>712</v>
       </c>
@@ -12461,7 +12466,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:42">
       <c r="A52" s="1" t="s">
         <v>723</v>
       </c>
@@ -12589,7 +12594,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:42">
       <c r="A53" s="1" t="s">
         <v>733</v>
       </c>
@@ -12717,7 +12722,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:42">
       <c r="A54" s="1" t="s">
         <v>745</v>
       </c>
@@ -12845,7 +12850,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:42">
       <c r="A55" s="1" t="s">
         <v>751</v>
       </c>
@@ -12973,7 +12978,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:42">
       <c r="A56" s="1" t="s">
         <v>765</v>
       </c>
@@ -13101,7 +13106,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:42">
       <c r="A57" s="1" t="s">
         <v>775</v>
       </c>
@@ -13229,7 +13234,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:42">
       <c r="A58" s="1" t="s">
         <v>788</v>
       </c>
@@ -13357,7 +13362,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:42">
       <c r="A59" s="1" t="s">
         <v>800</v>
       </c>
@@ -13485,7 +13490,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:42">
       <c r="A60" s="1" t="s">
         <v>807</v>
       </c>
@@ -13613,7 +13618,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:42">
       <c r="A61" s="1" t="s">
         <v>814</v>
       </c>
@@ -13741,7 +13746,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:42">
       <c r="A62" s="1" t="s">
         <v>825</v>
       </c>
@@ -13869,7 +13874,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="63" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:42">
       <c r="A63" s="1" t="s">
         <v>835</v>
       </c>
@@ -13997,7 +14002,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="64" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:42">
       <c r="A64" s="1" t="s">
         <v>847</v>
       </c>
@@ -14125,7 +14130,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:42">
       <c r="A65" s="1" t="s">
         <v>858</v>
       </c>
@@ -14253,7 +14258,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:42">
       <c r="A66" s="1" t="s">
         <v>867</v>
       </c>
@@ -14381,7 +14386,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:42">
       <c r="A67" s="1" t="s">
         <v>883</v>
       </c>
@@ -14509,7 +14514,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:42">
       <c r="A68" s="1" t="s">
         <v>899</v>
       </c>
@@ -14637,7 +14642,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:42">
       <c r="A69" s="1" t="s">
         <v>909</v>
       </c>
@@ -14765,7 +14770,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:42">
       <c r="A70" s="1" t="s">
         <v>918</v>
       </c>
@@ -14893,7 +14898,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:42">
       <c r="A71" s="1" t="s">
         <v>931</v>
       </c>
@@ -15021,7 +15026,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:42">
       <c r="A72" s="1" t="s">
         <v>945</v>
       </c>
@@ -15149,7 +15154,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:42">
       <c r="A73" s="1" t="s">
         <v>959</v>
       </c>
@@ -15277,7 +15282,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:42">
       <c r="A74" s="1" t="s">
         <v>971</v>
       </c>
@@ -15405,7 +15410,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:42">
       <c r="A75" s="1" t="s">
         <v>983</v>
       </c>
@@ -15533,7 +15538,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:42">
       <c r="A76" s="1" t="s">
         <v>992</v>
       </c>
@@ -15661,7 +15666,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:42">
       <c r="A77" s="1" t="s">
         <v>1003</v>
       </c>
@@ -15789,7 +15794,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:42">
       <c r="A78" s="1" t="s">
         <v>1012</v>
       </c>
@@ -15917,7 +15922,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:42">
       <c r="A79" s="1" t="s">
         <v>1026</v>
       </c>
@@ -16045,7 +16050,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:42">
       <c r="A80" s="1" t="s">
         <v>1039</v>
       </c>
@@ -16173,7 +16178,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:42">
       <c r="A81" s="1" t="s">
         <v>1048</v>
       </c>
@@ -16301,7 +16306,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:42">
       <c r="A82" s="1" t="s">
         <v>1061</v>
       </c>
@@ -16429,7 +16434,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="83" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:42">
       <c r="A83" s="1" t="s">
         <v>1074</v>
       </c>
@@ -16557,7 +16562,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="84" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:42">
       <c r="A84" s="1" t="s">
         <v>1086</v>
       </c>
@@ -16685,7 +16690,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:42">
       <c r="A85" s="1" t="s">
         <v>1101</v>
       </c>
@@ -16813,7 +16818,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:42">
       <c r="A86" s="1" t="s">
         <v>1114</v>
       </c>
@@ -16941,7 +16946,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:42">
       <c r="A87" s="1" t="s">
         <v>1131</v>
       </c>
@@ -17069,7 +17074,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:42">
       <c r="A88" s="1" t="s">
         <v>1144</v>
       </c>
@@ -17197,7 +17202,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:42">
       <c r="A89" s="1" t="s">
         <v>1156</v>
       </c>
@@ -17325,7 +17330,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:42">
       <c r="A90" s="1" t="s">
         <v>1164</v>
       </c>
@@ -17453,7 +17458,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:42">
       <c r="A91" s="1" t="s">
         <v>1173</v>
       </c>
@@ -17581,7 +17586,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:42">
       <c r="A92" s="1" t="s">
         <v>1182</v>
       </c>
@@ -17709,7 +17714,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:42">
       <c r="A93" s="1" t="s">
         <v>1195</v>
       </c>
@@ -17837,7 +17842,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:42">
       <c r="A94" s="1" t="s">
         <v>1209</v>
       </c>
@@ -17965,7 +17970,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:42">
       <c r="A95" s="1" t="s">
         <v>1211</v>
       </c>
@@ -18093,7 +18098,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:42">
       <c r="A96" s="1" t="s">
         <v>1225</v>
       </c>
@@ -18221,7 +18226,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="97" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:42">
       <c r="A97" s="1" t="s">
         <v>1235</v>
       </c>
@@ -18349,7 +18354,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="98" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:42">
       <c r="A98" s="1" t="s">
         <v>1246</v>
       </c>
@@ -18477,7 +18482,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="99" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:42">
       <c r="A99" s="1" t="s">
         <v>1255</v>
       </c>
@@ -18605,7 +18610,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="100" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:42">
       <c r="A100" s="1" t="s">
         <v>1266</v>
       </c>
@@ -18733,7 +18738,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="101" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:42">
       <c r="A101" s="1" t="s">
         <v>1276</v>
       </c>
@@ -18861,7 +18866,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="102" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:42">
       <c r="A102" s="1" t="s">
         <v>1288</v>
       </c>
@@ -18989,7 +18994,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="103" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:42">
       <c r="A103" s="1" t="s">
         <v>1302</v>
       </c>
@@ -19117,7 +19122,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="104" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:42">
       <c r="A104" s="1" t="s">
         <v>1314</v>
       </c>
@@ -19245,7 +19250,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="105" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:42">
       <c r="A105" s="1" t="s">
         <v>1325</v>
       </c>
@@ -19373,7 +19378,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="106" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:42">
       <c r="A106" s="1" t="s">
         <v>1339</v>
       </c>
@@ -19501,7 +19506,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:42">
       <c r="A107" s="1" t="s">
         <v>1348</v>
       </c>
@@ -19629,7 +19634,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="108" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:42">
       <c r="A108" s="1" t="s">
         <v>1359</v>
       </c>
@@ -19757,7 +19762,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="109" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:42">
       <c r="A109" s="1" t="s">
         <v>1370</v>
       </c>
@@ -19885,7 +19890,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="110" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:42">
       <c r="A110" s="1" t="s">
         <v>1380</v>
       </c>
@@ -20013,7 +20018,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="111" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:42">
       <c r="A111" s="1" t="s">
         <v>1393</v>
       </c>
@@ -20141,7 +20146,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="112" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:42">
       <c r="A112" s="1" t="s">
         <v>1406</v>
       </c>
@@ -20269,7 +20274,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="113" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:42">
       <c r="A113" s="1" t="s">
         <v>1420</v>
       </c>
@@ -20397,7 +20402,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="114" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:42">
       <c r="A114" s="1" t="s">
         <v>1436</v>
       </c>
@@ -20525,7 +20530,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="115" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:42">
       <c r="A115" s="1" t="s">
         <v>1449</v>
       </c>
@@ -20653,7 +20658,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="116" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:42">
       <c r="A116" s="1" t="s">
         <v>1459</v>
       </c>
@@ -20781,7 +20786,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="117" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:42">
       <c r="A117" s="1" t="s">
         <v>1471</v>
       </c>
@@ -20909,7 +20914,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="118" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:42">
       <c r="A118" s="1" t="s">
         <v>1477</v>
       </c>
@@ -21037,7 +21042,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="119" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:42">
       <c r="A119" s="1" t="s">
         <v>1488</v>
       </c>
@@ -21165,7 +21170,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="120" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:42">
       <c r="A120" s="1" t="s">
         <v>1505</v>
       </c>
@@ -21293,7 +21298,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="121" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:42">
       <c r="A121" s="1" t="s">
         <v>1514</v>
       </c>
@@ -21421,7 +21426,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="122" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:42">
       <c r="A122" s="1" t="s">
         <v>1525</v>
       </c>
@@ -21549,7 +21554,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="123" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:42">
       <c r="A123" s="1" t="s">
         <v>1536</v>
       </c>
@@ -21677,7 +21682,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:42">
       <c r="A124" s="1" t="s">
         <v>1548</v>
       </c>
@@ -21805,7 +21810,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:42">
       <c r="A125" s="1" t="s">
         <v>1560</v>
       </c>
@@ -21933,7 +21938,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:42">
       <c r="A126" s="1" t="s">
         <v>1575</v>
       </c>
@@ -22061,7 +22066,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="127" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:42">
       <c r="A127" s="1" t="s">
         <v>1584</v>
       </c>
@@ -22189,7 +22194,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="128" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:42">
       <c r="A128" s="1" t="s">
         <v>1595</v>
       </c>
@@ -22317,7 +22322,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="129" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:42">
       <c r="A129" s="1" t="s">
         <v>1607</v>
       </c>
@@ -22445,7 +22450,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="130" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:42">
       <c r="A130" s="1" t="s">
         <v>1614</v>
       </c>
@@ -22573,7 +22578,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="131" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:42">
       <c r="A131" s="1" t="s">
         <v>1623</v>
       </c>
@@ -22701,7 +22706,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="132" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:42">
       <c r="A132" s="1" t="s">
         <v>1630</v>
       </c>
@@ -22829,7 +22834,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="133" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:42">
       <c r="A133" s="1" t="s">
         <v>1638</v>
       </c>
@@ -22957,7 +22962,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="134" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:42">
       <c r="A134" s="1" t="s">
         <v>1647</v>
       </c>
@@ -23085,7 +23090,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="135" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:42">
       <c r="A135" s="1" t="s">
         <v>1663</v>
       </c>
@@ -23213,7 +23218,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="136" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:42">
       <c r="A136" s="1" t="s">
         <v>1676</v>
       </c>
@@ -23341,7 +23346,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="137" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:42">
       <c r="A137" s="1" t="s">
         <v>1688</v>
       </c>
@@ -23469,7 +23474,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="138" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:42">
       <c r="A138" s="1" t="s">
         <v>1702</v>
       </c>
@@ -23597,7 +23602,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="139" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:42">
       <c r="A139" s="1" t="s">
         <v>1713</v>
       </c>
@@ -23725,7 +23730,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="140" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:42">
       <c r="A140" s="1" t="s">
         <v>1722</v>
       </c>
@@ -23853,7 +23858,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="141" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:42">
       <c r="A141" s="1" t="s">
         <v>1733</v>
       </c>
@@ -23981,7 +23986,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="142" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:42">
       <c r="A142" s="1" t="s">
         <v>1744</v>
       </c>
@@ -24109,7 +24114,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="143" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:42">
       <c r="A143" s="1" t="s">
         <v>1760</v>
       </c>
@@ -24237,7 +24242,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="144" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:42">
       <c r="A144" s="1" t="s">
         <v>1766</v>
       </c>
@@ -24365,7 +24370,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="145" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:42">
       <c r="A145" s="1" t="s">
         <v>1778</v>
       </c>
@@ -24493,7 +24498,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="146" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:42">
       <c r="A146" s="1" t="s">
         <v>1793</v>
       </c>
@@ -24621,7 +24626,7 @@
         <v>1806</v>
       </c>
     </row>
-    <row r="147" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:42">
       <c r="A147" s="1" t="s">
         <v>1807</v>
       </c>
@@ -24749,7 +24754,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="148" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:42">
       <c r="A148" s="1" t="s">
         <v>1817</v>
       </c>
@@ -24877,7 +24882,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="149" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:42">
       <c r="A149" s="1" t="s">
         <v>1825</v>
       </c>
@@ -25005,7 +25010,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="150" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:42">
       <c r="A150" s="1" t="s">
         <v>1837</v>
       </c>
@@ -25135,6 +25140,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -25144,9 +25154,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -25156,8 +25171,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>